<commit_message>
feat: RDCC-3540 Modified test files
</commit_message>
<xml_diff>
--- a/src/test/resources/Staff Data Upload With Empty Rows.xlsx
+++ b/src/test/resources/Staff Data Upload With Empty Rows.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF2A4722-40CE-8347-B1AD-442C948FA3CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85BF11E-EAB8-0F4A-AB80-5248E24E8101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="3" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="VERSION" sheetId="13" r:id="rId1"/>
     <sheet name="Guidance" sheetId="16" r:id="rId2"/>
     <sheet name="Terminology" sheetId="12" r:id="rId3"/>
-    <sheet name="Case Worker Data" sheetId="1" r:id="rId4"/>
+    <sheet name="Staff Data" sheetId="1" r:id="rId4"/>
     <sheet name="User Type" sheetId="9" state="hidden" r:id="rId5"/>
     <sheet name="Services" sheetId="7" state="hidden" r:id="rId6"/>
     <sheet name="Base Locations" sheetId="6" state="hidden" r:id="rId7"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="1236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="1244">
   <si>
     <t>Region</t>
   </si>
@@ -3389,30 +3389,6 @@
   </si>
   <si>
     <t>Primary Base Location ID</t>
-  </si>
-  <si>
-    <t>Area of Work2 ID</t>
-  </si>
-  <si>
-    <t>Area of Work1 ID</t>
-  </si>
-  <si>
-    <t>Area of Work3 ID</t>
-  </si>
-  <si>
-    <t>Area of Work4 ID</t>
-  </si>
-  <si>
-    <t>Area of Work5 ID</t>
-  </si>
-  <si>
-    <t>Area of Work6 ID</t>
-  </si>
-  <si>
-    <t>Area of Work7 ID</t>
-  </si>
-  <si>
-    <t>Area of Work8 ID</t>
   </si>
   <si>
     <t>Suspended</t>
@@ -3885,6 +3861,54 @@
   </si>
   <si>
     <t xml:space="preserve">https://github.com/hmcts/rpx-xui-approve-org/blob/master/staff/Staff_Data_Upload_Template.xlsx. </t>
+  </si>
+  <si>
+    <t>Service1</t>
+  </si>
+  <si>
+    <t>Service1 ID</t>
+  </si>
+  <si>
+    <t>Service2</t>
+  </si>
+  <si>
+    <t>Service2 ID</t>
+  </si>
+  <si>
+    <t>Service3</t>
+  </si>
+  <si>
+    <t>Service3 ID</t>
+  </si>
+  <si>
+    <t>Service4</t>
+  </si>
+  <si>
+    <t>Service4 ID</t>
+  </si>
+  <si>
+    <t>Service5</t>
+  </si>
+  <si>
+    <t>Service5 ID</t>
+  </si>
+  <si>
+    <t>Service6</t>
+  </si>
+  <si>
+    <t>Service6 ID</t>
+  </si>
+  <si>
+    <t>Service7</t>
+  </si>
+  <si>
+    <t>Service7 ID</t>
+  </si>
+  <si>
+    <t>Service8</t>
+  </si>
+  <si>
+    <t>Service8 ID</t>
   </si>
 </sst>
 </file>
@@ -4450,19 +4474,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4470,12 +4482,24 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -12861,7 +12885,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
-        <v>1199</v>
+        <v>1191</v>
       </c>
       <c r="B1" s="43"/>
       <c r="C1" s="43"/>
@@ -12875,17 +12899,17 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
-        <v>1196</v>
+        <v>1188</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>1202</v>
+        <v>1194</v>
       </c>
       <c r="C3" s="46"/>
       <c r="D3" s="47"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="48" t="s">
-        <v>1197</v>
+        <v>1189</v>
       </c>
       <c r="B4" s="53">
         <v>2021</v>
@@ -12895,20 +12919,20 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
-        <v>1198</v>
+        <v>1190</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>1201</v>
+        <v>1193</v>
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="47"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
-        <v>1200</v>
+        <v>1192</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>1234</v>
+        <v>1226</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="47"/>
@@ -12979,7 +13003,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1121</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -13104,20 +13128,20 @@
     </row>
     <row r="4" spans="1:34" s="70" customFormat="1" ht="34.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="68"/>
-      <c r="B4" s="76" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
+      <c r="B4" s="72" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
       <c r="J4" s="68"/>
       <c r="K4" s="68"/>
       <c r="L4" s="67" t="s">
-        <v>1209</v>
+        <v>1201</v>
       </c>
       <c r="M4" s="68"/>
       <c r="N4" s="68"/>
@@ -13128,16 +13152,16 @@
       <c r="S4" s="68"/>
       <c r="T4" s="68"/>
       <c r="U4" s="68"/>
-      <c r="V4" s="76" t="s">
-        <v>1210</v>
-      </c>
-      <c r="W4" s="76"/>
-      <c r="X4" s="76"/>
-      <c r="Y4" s="76"/>
-      <c r="Z4" s="76"/>
-      <c r="AA4" s="76"/>
-      <c r="AB4" s="76"/>
-      <c r="AC4" s="76"/>
+      <c r="V4" s="72" t="s">
+        <v>1202</v>
+      </c>
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+      <c r="AC4" s="72"/>
       <c r="AD4" s="69"/>
       <c r="AE4" s="69"/>
       <c r="AF4" s="69"/>
@@ -13146,16 +13170,16 @@
     </row>
     <row r="5" spans="1:34" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30"/>
-      <c r="B5" s="77" t="s">
-        <v>1235</v>
-      </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
+      <c r="B5" s="73" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
       <c r="J5" s="30"/>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -13168,16 +13192,16 @@
       <c r="S5" s="30"/>
       <c r="T5" s="30"/>
       <c r="U5" s="30"/>
-      <c r="V5" s="78" t="s">
-        <v>1211</v>
-      </c>
-      <c r="W5" s="71"/>
-      <c r="X5" s="71"/>
-      <c r="Y5" s="71"/>
-      <c r="Z5" s="71"/>
-      <c r="AA5" s="71"/>
-      <c r="AB5" s="71"/>
-      <c r="AC5" s="71"/>
+      <c r="V5" s="75" t="s">
+        <v>1203</v>
+      </c>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
+      <c r="Z5" s="74"/>
+      <c r="AA5" s="74"/>
+      <c r="AB5" s="74"/>
+      <c r="AC5" s="74"/>
     </row>
     <row r="6" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="30"/>
@@ -13212,16 +13236,16 @@
     </row>
     <row r="7" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="30"/>
-      <c r="B7" s="79" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79"/>
+      <c r="B7" s="76" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
@@ -13234,29 +13258,29 @@
       <c r="S7" s="30"/>
       <c r="T7" s="30"/>
       <c r="U7" s="30"/>
-      <c r="V7" s="79" t="s">
-        <v>1213</v>
-      </c>
-      <c r="W7" s="79"/>
-      <c r="X7" s="79"/>
-      <c r="Y7" s="79"/>
-      <c r="Z7" s="79"/>
-      <c r="AA7" s="79"/>
-      <c r="AB7" s="79"/>
-      <c r="AC7" s="79"/>
+      <c r="V7" s="76" t="s">
+        <v>1205</v>
+      </c>
+      <c r="W7" s="76"/>
+      <c r="X7" s="76"/>
+      <c r="Y7" s="76"/>
+      <c r="Z7" s="76"/>
+      <c r="AA7" s="76"/>
+      <c r="AB7" s="76"/>
+      <c r="AC7" s="76"/>
     </row>
     <row r="8" spans="1:34" ht="32.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30"/>
-      <c r="B8" s="73" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
+      <c r="B8" s="77" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -13269,16 +13293,16 @@
       <c r="S8" s="30"/>
       <c r="T8" s="30"/>
       <c r="U8" s="30"/>
-      <c r="V8" s="73" t="s">
-        <v>1215</v>
-      </c>
-      <c r="W8" s="73"/>
-      <c r="X8" s="73"/>
-      <c r="Y8" s="73"/>
-      <c r="Z8" s="73"/>
-      <c r="AA8" s="73"/>
-      <c r="AB8" s="73"/>
-      <c r="AC8" s="73"/>
+      <c r="V8" s="77" t="s">
+        <v>1207</v>
+      </c>
+      <c r="W8" s="77"/>
+      <c r="X8" s="77"/>
+      <c r="Y8" s="77"/>
+      <c r="Z8" s="77"/>
+      <c r="AA8" s="77"/>
+      <c r="AB8" s="77"/>
+      <c r="AC8" s="77"/>
     </row>
     <row r="9" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="30"/>
@@ -13333,16 +13357,16 @@
       <c r="S10" s="30"/>
       <c r="T10" s="30"/>
       <c r="U10" s="30"/>
-      <c r="V10" s="73" t="s">
-        <v>1216</v>
-      </c>
-      <c r="W10" s="73"/>
-      <c r="X10" s="73"/>
-      <c r="Y10" s="73"/>
-      <c r="Z10" s="73"/>
-      <c r="AA10" s="73"/>
-      <c r="AB10" s="73"/>
-      <c r="AC10" s="73"/>
+      <c r="V10" s="77" t="s">
+        <v>1208</v>
+      </c>
+      <c r="W10" s="77"/>
+      <c r="X10" s="77"/>
+      <c r="Y10" s="77"/>
+      <c r="Z10" s="77"/>
+      <c r="AA10" s="77"/>
+      <c r="AB10" s="77"/>
+      <c r="AC10" s="77"/>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="30"/>
@@ -13511,16 +13535,16 @@
       <c r="I16" s="30"/>
       <c r="J16" s="30"/>
       <c r="K16" s="30"/>
-      <c r="L16" s="74" t="s">
-        <v>1217</v>
-      </c>
-      <c r="M16" s="74"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74"/>
-      <c r="S16" s="74"/>
+      <c r="L16" s="71" t="s">
+        <v>1209</v>
+      </c>
+      <c r="M16" s="71"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="71"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
       <c r="T16" s="30"/>
       <c r="U16" s="30"/>
       <c r="V16" s="30"/>
@@ -13544,14 +13568,14 @@
       <c r="I17" s="30"/>
       <c r="J17" s="30"/>
       <c r="K17" s="30"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="74"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
       <c r="T17" s="30"/>
       <c r="U17" s="30"/>
       <c r="V17" s="30"/>
@@ -13575,16 +13599,16 @@
       <c r="I18" s="30"/>
       <c r="J18" s="30"/>
       <c r="K18" s="30"/>
-      <c r="L18" s="80" t="s">
-        <v>1218</v>
-      </c>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="75"/>
-      <c r="R18" s="75"/>
-      <c r="S18" s="75"/>
+      <c r="L18" s="78" t="s">
+        <v>1210</v>
+      </c>
+      <c r="M18" s="79"/>
+      <c r="N18" s="79"/>
+      <c r="O18" s="79"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="79"/>
+      <c r="R18" s="79"/>
+      <c r="S18" s="79"/>
       <c r="T18" s="30"/>
       <c r="U18" s="30"/>
       <c r="V18" s="30"/>
@@ -13639,16 +13663,16 @@
       <c r="I20" s="30"/>
       <c r="J20" s="30"/>
       <c r="K20" s="30"/>
-      <c r="L20" s="74" t="s">
-        <v>1219</v>
-      </c>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="74"/>
-      <c r="S20" s="74"/>
+      <c r="L20" s="71" t="s">
+        <v>1211</v>
+      </c>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="71"/>
+      <c r="Q20" s="71"/>
+      <c r="R20" s="71"/>
+      <c r="S20" s="71"/>
       <c r="T20" s="30"/>
       <c r="U20" s="30"/>
       <c r="V20" s="30"/>
@@ -13672,14 +13696,14 @@
       <c r="I21" s="30"/>
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="74"/>
-      <c r="Q21" s="74"/>
-      <c r="R21" s="74"/>
-      <c r="S21" s="74"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="71"/>
+      <c r="Q21" s="71"/>
+      <c r="R21" s="71"/>
+      <c r="S21" s="71"/>
       <c r="T21" s="30"/>
       <c r="U21" s="30"/>
       <c r="V21" s="30"/>
@@ -13734,16 +13758,16 @@
       <c r="I23" s="30"/>
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
-      <c r="L23" s="72" t="s">
-        <v>1220</v>
-      </c>
-      <c r="M23" s="72"/>
-      <c r="N23" s="72"/>
-      <c r="O23" s="72"/>
-      <c r="P23" s="72"/>
-      <c r="Q23" s="72"/>
-      <c r="R23" s="72"/>
-      <c r="S23" s="72"/>
+      <c r="L23" s="80" t="s">
+        <v>1212</v>
+      </c>
+      <c r="M23" s="80"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="80"/>
+      <c r="S23" s="80"/>
       <c r="T23" s="30"/>
       <c r="U23" s="30"/>
       <c r="V23" s="30"/>
@@ -13767,14 +13791,14 @@
       <c r="I24" s="30"/>
       <c r="J24" s="30"/>
       <c r="K24" s="30"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="72"/>
-      <c r="P24" s="72"/>
-      <c r="Q24" s="72"/>
-      <c r="R24" s="72"/>
-      <c r="S24" s="72"/>
+      <c r="L24" s="80"/>
+      <c r="M24" s="80"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="80"/>
+      <c r="P24" s="80"/>
+      <c r="Q24" s="80"/>
+      <c r="R24" s="80"/>
+      <c r="S24" s="80"/>
       <c r="T24" s="30"/>
       <c r="U24" s="30"/>
       <c r="V24" s="30"/>
@@ -13944,40 +13968,40 @@
     </row>
     <row r="31" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="30"/>
-      <c r="B31" s="73" t="s">
-        <v>1221</v>
-      </c>
-      <c r="C31" s="73"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="73"/>
-      <c r="I31" s="73"/>
+      <c r="B31" s="77" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
       <c r="J31" s="30"/>
       <c r="K31" s="30"/>
-      <c r="L31" s="74" t="s">
-        <v>1222</v>
-      </c>
-      <c r="M31" s="74"/>
-      <c r="N31" s="74"/>
-      <c r="O31" s="74"/>
-      <c r="P31" s="74"/>
-      <c r="Q31" s="74"/>
-      <c r="R31" s="74"/>
-      <c r="S31" s="74"/>
+      <c r="L31" s="71" t="s">
+        <v>1214</v>
+      </c>
+      <c r="M31" s="71"/>
+      <c r="N31" s="71"/>
+      <c r="O31" s="71"/>
+      <c r="P31" s="71"/>
+      <c r="Q31" s="71"/>
+      <c r="R31" s="71"/>
+      <c r="S31" s="71"/>
       <c r="T31" s="30"/>
       <c r="U31" s="30"/>
-      <c r="V31" s="74" t="s">
-        <v>1223</v>
-      </c>
-      <c r="W31" s="75"/>
-      <c r="X31" s="75"/>
-      <c r="Y31" s="75"/>
-      <c r="Z31" s="75"/>
-      <c r="AA31" s="75"/>
-      <c r="AB31" s="75"/>
-      <c r="AC31" s="75"/>
+      <c r="V31" s="71" t="s">
+        <v>1215</v>
+      </c>
+      <c r="W31" s="79"/>
+      <c r="X31" s="79"/>
+      <c r="Y31" s="79"/>
+      <c r="Z31" s="79"/>
+      <c r="AA31" s="79"/>
+      <c r="AB31" s="79"/>
+      <c r="AC31" s="79"/>
     </row>
     <row r="32" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="30"/>
@@ -13991,68 +14015,68 @@
       <c r="I32" s="30"/>
       <c r="J32" s="30"/>
       <c r="K32" s="30"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="74"/>
-      <c r="R32" s="74"/>
-      <c r="S32" s="74"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="71"/>
+      <c r="N32" s="71"/>
+      <c r="O32" s="71"/>
+      <c r="P32" s="71"/>
+      <c r="Q32" s="71"/>
+      <c r="R32" s="71"/>
+      <c r="S32" s="71"/>
       <c r="T32" s="30"/>
       <c r="U32" s="30"/>
-      <c r="V32" s="75"/>
-      <c r="W32" s="75"/>
-      <c r="X32" s="75"/>
-      <c r="Y32" s="75"/>
-      <c r="Z32" s="75"/>
-      <c r="AA32" s="75"/>
-      <c r="AB32" s="75"/>
-      <c r="AC32" s="75"/>
+      <c r="V32" s="79"/>
+      <c r="W32" s="79"/>
+      <c r="X32" s="79"/>
+      <c r="Y32" s="79"/>
+      <c r="Z32" s="79"/>
+      <c r="AA32" s="79"/>
+      <c r="AB32" s="79"/>
+      <c r="AC32" s="79"/>
     </row>
     <row r="33" spans="1:29" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="30"/>
-      <c r="B33" s="71" t="s">
-        <v>1224</v>
-      </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
+      <c r="B33" s="74" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
       <c r="J33" s="30"/>
       <c r="K33" s="30"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+      <c r="N33" s="71"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="71"/>
+      <c r="Q33" s="71"/>
+      <c r="R33" s="71"/>
+      <c r="S33" s="71"/>
       <c r="T33" s="30"/>
       <c r="U33" s="30"/>
-      <c r="V33" s="75"/>
-      <c r="W33" s="75"/>
-      <c r="X33" s="75"/>
-      <c r="Y33" s="75"/>
-      <c r="Z33" s="75"/>
-      <c r="AA33" s="75"/>
-      <c r="AB33" s="75"/>
-      <c r="AC33" s="75"/>
+      <c r="V33" s="79"/>
+      <c r="W33" s="79"/>
+      <c r="X33" s="79"/>
+      <c r="Y33" s="79"/>
+      <c r="Z33" s="79"/>
+      <c r="AA33" s="79"/>
+      <c r="AB33" s="79"/>
+      <c r="AC33" s="79"/>
     </row>
     <row r="34" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
       <c r="J34" s="30"/>
       <c r="K34" s="30"/>
       <c r="L34" s="30"/>
@@ -14086,28 +14110,28 @@
       <c r="I35" s="30"/>
       <c r="J35" s="30"/>
       <c r="K35" s="30"/>
-      <c r="L35" s="74" t="s">
-        <v>1225</v>
-      </c>
-      <c r="M35" s="74"/>
-      <c r="N35" s="74"/>
-      <c r="O35" s="74"/>
-      <c r="P35" s="74"/>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="74"/>
-      <c r="S35" s="74"/>
+      <c r="L35" s="71" t="s">
+        <v>1217</v>
+      </c>
+      <c r="M35" s="71"/>
+      <c r="N35" s="71"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="71"/>
+      <c r="Q35" s="71"/>
+      <c r="R35" s="71"/>
+      <c r="S35" s="71"/>
       <c r="T35" s="30"/>
       <c r="U35" s="30"/>
-      <c r="V35" s="71" t="s">
-        <v>1226</v>
-      </c>
-      <c r="W35" s="71"/>
-      <c r="X35" s="71"/>
-      <c r="Y35" s="71"/>
-      <c r="Z35" s="71"/>
-      <c r="AA35" s="71"/>
-      <c r="AB35" s="71"/>
-      <c r="AC35" s="71"/>
+      <c r="V35" s="74" t="s">
+        <v>1218</v>
+      </c>
+      <c r="W35" s="74"/>
+      <c r="X35" s="74"/>
+      <c r="Y35" s="74"/>
+      <c r="Z35" s="74"/>
+      <c r="AA35" s="74"/>
+      <c r="AB35" s="74"/>
+      <c r="AC35" s="74"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="30"/>
@@ -14121,24 +14145,24 @@
       <c r="I36" s="30"/>
       <c r="J36" s="30"/>
       <c r="K36" s="30"/>
-      <c r="L36" s="74"/>
-      <c r="M36" s="74"/>
-      <c r="N36" s="74"/>
-      <c r="O36" s="74"/>
-      <c r="P36" s="74"/>
-      <c r="Q36" s="74"/>
-      <c r="R36" s="74"/>
-      <c r="S36" s="74"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="71"/>
+      <c r="N36" s="71"/>
+      <c r="O36" s="71"/>
+      <c r="P36" s="71"/>
+      <c r="Q36" s="71"/>
+      <c r="R36" s="71"/>
+      <c r="S36" s="71"/>
       <c r="T36" s="30"/>
       <c r="U36" s="30"/>
-      <c r="V36" s="71"/>
-      <c r="W36" s="71"/>
-      <c r="X36" s="71"/>
-      <c r="Y36" s="71"/>
-      <c r="Z36" s="71"/>
-      <c r="AA36" s="71"/>
-      <c r="AB36" s="71"/>
-      <c r="AC36" s="71"/>
+      <c r="V36" s="74"/>
+      <c r="W36" s="74"/>
+      <c r="X36" s="74"/>
+      <c r="Y36" s="74"/>
+      <c r="Z36" s="74"/>
+      <c r="AA36" s="74"/>
+      <c r="AB36" s="74"/>
+      <c r="AC36" s="74"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="30"/>
@@ -14152,14 +14176,14 @@
       <c r="I37" s="30"/>
       <c r="J37" s="30"/>
       <c r="K37" s="30"/>
-      <c r="L37" s="74"/>
-      <c r="M37" s="74"/>
-      <c r="N37" s="74"/>
-      <c r="O37" s="74"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="74"/>
-      <c r="R37" s="74"/>
-      <c r="S37" s="74"/>
+      <c r="L37" s="71"/>
+      <c r="M37" s="71"/>
+      <c r="N37" s="71"/>
+      <c r="O37" s="71"/>
+      <c r="P37" s="71"/>
+      <c r="Q37" s="71"/>
+      <c r="R37" s="71"/>
+      <c r="S37" s="71"/>
       <c r="T37" s="30"/>
       <c r="U37" s="30"/>
       <c r="V37" s="30"/>
@@ -14183,26 +14207,26 @@
       <c r="I38" s="30"/>
       <c r="J38" s="30"/>
       <c r="K38" s="30"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="74"/>
-      <c r="R38" s="74"/>
-      <c r="S38" s="74"/>
+      <c r="L38" s="71"/>
+      <c r="M38" s="71"/>
+      <c r="N38" s="71"/>
+      <c r="O38" s="71"/>
+      <c r="P38" s="71"/>
+      <c r="Q38" s="71"/>
+      <c r="R38" s="71"/>
+      <c r="S38" s="71"/>
       <c r="T38" s="30"/>
       <c r="U38" s="30"/>
-      <c r="V38" s="72" t="s">
-        <v>1219</v>
-      </c>
-      <c r="W38" s="72"/>
-      <c r="X38" s="72"/>
-      <c r="Y38" s="72"/>
-      <c r="Z38" s="72"/>
-      <c r="AA38" s="72"/>
-      <c r="AB38" s="72"/>
-      <c r="AC38" s="72"/>
+      <c r="V38" s="80" t="s">
+        <v>1211</v>
+      </c>
+      <c r="W38" s="80"/>
+      <c r="X38" s="80"/>
+      <c r="Y38" s="80"/>
+      <c r="Z38" s="80"/>
+      <c r="AA38" s="80"/>
+      <c r="AB38" s="80"/>
+      <c r="AC38" s="80"/>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="30"/>
@@ -14216,26 +14240,26 @@
       <c r="I39" s="30"/>
       <c r="J39" s="30"/>
       <c r="K39" s="30"/>
-      <c r="L39" s="74" t="s">
-        <v>1227</v>
-      </c>
-      <c r="M39" s="74"/>
-      <c r="N39" s="74"/>
-      <c r="O39" s="74"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="74"/>
-      <c r="R39" s="74"/>
-      <c r="S39" s="74"/>
+      <c r="L39" s="71" t="s">
+        <v>1219</v>
+      </c>
+      <c r="M39" s="71"/>
+      <c r="N39" s="71"/>
+      <c r="O39" s="71"/>
+      <c r="P39" s="71"/>
+      <c r="Q39" s="71"/>
+      <c r="R39" s="71"/>
+      <c r="S39" s="71"/>
       <c r="T39" s="30"/>
       <c r="U39" s="30"/>
-      <c r="V39" s="72"/>
-      <c r="W39" s="72"/>
-      <c r="X39" s="72"/>
-      <c r="Y39" s="72"/>
-      <c r="Z39" s="72"/>
-      <c r="AA39" s="72"/>
-      <c r="AB39" s="72"/>
-      <c r="AC39" s="72"/>
+      <c r="V39" s="80"/>
+      <c r="W39" s="80"/>
+      <c r="X39" s="80"/>
+      <c r="Y39" s="80"/>
+      <c r="Z39" s="80"/>
+      <c r="AA39" s="80"/>
+      <c r="AB39" s="80"/>
+      <c r="AC39" s="80"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="30"/>
@@ -14249,14 +14273,14 @@
       <c r="I40" s="30"/>
       <c r="J40" s="30"/>
       <c r="K40" s="30"/>
-      <c r="L40" s="74"/>
-      <c r="M40" s="74"/>
-      <c r="N40" s="74"/>
-      <c r="O40" s="74"/>
-      <c r="P40" s="74"/>
-      <c r="Q40" s="74"/>
-      <c r="R40" s="74"/>
-      <c r="S40" s="74"/>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71"/>
+      <c r="N40" s="71"/>
+      <c r="O40" s="71"/>
+      <c r="P40" s="71"/>
+      <c r="Q40" s="71"/>
+      <c r="R40" s="71"/>
+      <c r="S40" s="71"/>
       <c r="T40" s="30"/>
       <c r="U40" s="30"/>
       <c r="V40" s="30"/>
@@ -14280,28 +14304,28 @@
       <c r="I41" s="30"/>
       <c r="J41" s="30"/>
       <c r="K41" s="30"/>
-      <c r="L41" s="74" t="s">
-        <v>1228</v>
-      </c>
-      <c r="M41" s="74"/>
-      <c r="N41" s="74"/>
-      <c r="O41" s="74"/>
-      <c r="P41" s="74"/>
-      <c r="Q41" s="74"/>
-      <c r="R41" s="74"/>
-      <c r="S41" s="74"/>
+      <c r="L41" s="71" t="s">
+        <v>1220</v>
+      </c>
+      <c r="M41" s="71"/>
+      <c r="N41" s="71"/>
+      <c r="O41" s="71"/>
+      <c r="P41" s="71"/>
+      <c r="Q41" s="71"/>
+      <c r="R41" s="71"/>
+      <c r="S41" s="71"/>
       <c r="T41" s="30"/>
       <c r="U41" s="30"/>
-      <c r="V41" s="74" t="s">
-        <v>1229</v>
-      </c>
-      <c r="W41" s="74"/>
-      <c r="X41" s="74"/>
-      <c r="Y41" s="74"/>
-      <c r="Z41" s="74"/>
-      <c r="AA41" s="74"/>
-      <c r="AB41" s="74"/>
-      <c r="AC41" s="74"/>
+      <c r="V41" s="71" t="s">
+        <v>1221</v>
+      </c>
+      <c r="W41" s="71"/>
+      <c r="X41" s="71"/>
+      <c r="Y41" s="71"/>
+      <c r="Z41" s="71"/>
+      <c r="AA41" s="71"/>
+      <c r="AB41" s="71"/>
+      <c r="AC41" s="71"/>
     </row>
     <row r="42" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="30"/>
@@ -14315,24 +14339,24 @@
       <c r="I42" s="30"/>
       <c r="J42" s="30"/>
       <c r="K42" s="30"/>
-      <c r="L42" s="74"/>
-      <c r="M42" s="74"/>
-      <c r="N42" s="74"/>
-      <c r="O42" s="74"/>
-      <c r="P42" s="74"/>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="74"/>
-      <c r="S42" s="74"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
+      <c r="N42" s="71"/>
+      <c r="O42" s="71"/>
+      <c r="P42" s="71"/>
+      <c r="Q42" s="71"/>
+      <c r="R42" s="71"/>
+      <c r="S42" s="71"/>
       <c r="T42" s="30"/>
       <c r="U42" s="30"/>
-      <c r="V42" s="74"/>
-      <c r="W42" s="74"/>
-      <c r="X42" s="74"/>
-      <c r="Y42" s="74"/>
-      <c r="Z42" s="74"/>
-      <c r="AA42" s="74"/>
-      <c r="AB42" s="74"/>
-      <c r="AC42" s="74"/>
+      <c r="V42" s="71"/>
+      <c r="W42" s="71"/>
+      <c r="X42" s="71"/>
+      <c r="Y42" s="71"/>
+      <c r="Z42" s="71"/>
+      <c r="AA42" s="71"/>
+      <c r="AB42" s="71"/>
+      <c r="AC42" s="71"/>
     </row>
     <row r="43" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="30"/>
@@ -14346,26 +14370,26 @@
       <c r="I43" s="30"/>
       <c r="J43" s="30"/>
       <c r="K43" s="30"/>
-      <c r="L43" s="72" t="s">
-        <v>1230</v>
-      </c>
-      <c r="M43" s="72"/>
-      <c r="N43" s="72"/>
-      <c r="O43" s="72"/>
-      <c r="P43" s="72"/>
-      <c r="Q43" s="72"/>
-      <c r="R43" s="72"/>
-      <c r="S43" s="72"/>
+      <c r="L43" s="80" t="s">
+        <v>1222</v>
+      </c>
+      <c r="M43" s="80"/>
+      <c r="N43" s="80"/>
+      <c r="O43" s="80"/>
+      <c r="P43" s="80"/>
+      <c r="Q43" s="80"/>
+      <c r="R43" s="80"/>
+      <c r="S43" s="80"/>
       <c r="T43" s="30"/>
       <c r="U43" s="30"/>
-      <c r="V43" s="74"/>
-      <c r="W43" s="74"/>
-      <c r="X43" s="74"/>
-      <c r="Y43" s="74"/>
-      <c r="Z43" s="74"/>
-      <c r="AA43" s="74"/>
-      <c r="AB43" s="74"/>
-      <c r="AC43" s="74"/>
+      <c r="V43" s="71"/>
+      <c r="W43" s="71"/>
+      <c r="X43" s="71"/>
+      <c r="Y43" s="71"/>
+      <c r="Z43" s="71"/>
+      <c r="AA43" s="71"/>
+      <c r="AB43" s="71"/>
+      <c r="AC43" s="71"/>
     </row>
     <row r="44" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
@@ -14379,26 +14403,26 @@
       <c r="I44" s="30"/>
       <c r="J44" s="30"/>
       <c r="K44" s="30"/>
-      <c r="L44" s="72"/>
-      <c r="M44" s="72"/>
-      <c r="N44" s="72"/>
-      <c r="O44" s="72"/>
-      <c r="P44" s="72"/>
-      <c r="Q44" s="72"/>
-      <c r="R44" s="72"/>
-      <c r="S44" s="72"/>
+      <c r="L44" s="80"/>
+      <c r="M44" s="80"/>
+      <c r="N44" s="80"/>
+      <c r="O44" s="80"/>
+      <c r="P44" s="80"/>
+      <c r="Q44" s="80"/>
+      <c r="R44" s="80"/>
+      <c r="S44" s="80"/>
       <c r="T44" s="30"/>
       <c r="U44" s="30"/>
-      <c r="V44" s="71" t="s">
-        <v>1231</v>
-      </c>
-      <c r="W44" s="71"/>
-      <c r="X44" s="71"/>
-      <c r="Y44" s="71"/>
-      <c r="Z44" s="71"/>
-      <c r="AA44" s="71"/>
-      <c r="AB44" s="71"/>
-      <c r="AC44" s="71"/>
+      <c r="V44" s="74" t="s">
+        <v>1223</v>
+      </c>
+      <c r="W44" s="74"/>
+      <c r="X44" s="74"/>
+      <c r="Y44" s="74"/>
+      <c r="Z44" s="74"/>
+      <c r="AA44" s="74"/>
+      <c r="AB44" s="74"/>
+      <c r="AC44" s="74"/>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="30"/>
@@ -14412,24 +14436,24 @@
       <c r="I45" s="30"/>
       <c r="J45" s="30"/>
       <c r="K45" s="30"/>
-      <c r="L45" s="72"/>
-      <c r="M45" s="72"/>
-      <c r="N45" s="72"/>
-      <c r="O45" s="72"/>
-      <c r="P45" s="72"/>
-      <c r="Q45" s="72"/>
-      <c r="R45" s="72"/>
-      <c r="S45" s="72"/>
+      <c r="L45" s="80"/>
+      <c r="M45" s="80"/>
+      <c r="N45" s="80"/>
+      <c r="O45" s="80"/>
+      <c r="P45" s="80"/>
+      <c r="Q45" s="80"/>
+      <c r="R45" s="80"/>
+      <c r="S45" s="80"/>
       <c r="T45" s="30"/>
       <c r="U45" s="30"/>
-      <c r="V45" s="71"/>
-      <c r="W45" s="71"/>
-      <c r="X45" s="71"/>
-      <c r="Y45" s="71"/>
-      <c r="Z45" s="71"/>
-      <c r="AA45" s="71"/>
-      <c r="AB45" s="71"/>
-      <c r="AC45" s="71"/>
+      <c r="V45" s="74"/>
+      <c r="W45" s="74"/>
+      <c r="X45" s="74"/>
+      <c r="Y45" s="74"/>
+      <c r="Z45" s="74"/>
+      <c r="AA45" s="74"/>
+      <c r="AB45" s="74"/>
+      <c r="AC45" s="74"/>
     </row>
     <row r="46" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="30"/>
@@ -14443,16 +14467,16 @@
       <c r="I46" s="30"/>
       <c r="J46" s="30"/>
       <c r="K46" s="30"/>
-      <c r="L46" s="74" t="s">
-        <v>1232</v>
-      </c>
-      <c r="M46" s="74"/>
-      <c r="N46" s="74"/>
-      <c r="O46" s="74"/>
-      <c r="P46" s="74"/>
-      <c r="Q46" s="74"/>
-      <c r="R46" s="74"/>
-      <c r="S46" s="74"/>
+      <c r="L46" s="71" t="s">
+        <v>1224</v>
+      </c>
+      <c r="M46" s="71"/>
+      <c r="N46" s="71"/>
+      <c r="O46" s="71"/>
+      <c r="P46" s="71"/>
+      <c r="Q46" s="71"/>
+      <c r="R46" s="71"/>
+      <c r="S46" s="71"/>
       <c r="T46" s="30"/>
       <c r="U46" s="30"/>
       <c r="V46" s="30"/>
@@ -14466,26 +14490,26 @@
     </row>
     <row r="47" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
-      <c r="B47" s="71" t="s">
-        <v>1233</v>
-      </c>
-      <c r="C47" s="71"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="71"/>
-      <c r="H47" s="71"/>
-      <c r="I47" s="71"/>
+      <c r="B47" s="74" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C47" s="74"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="74"/>
+      <c r="H47" s="74"/>
+      <c r="I47" s="74"/>
       <c r="J47" s="30"/>
       <c r="K47" s="30"/>
-      <c r="L47" s="74"/>
-      <c r="M47" s="74"/>
-      <c r="N47" s="74"/>
-      <c r="O47" s="74"/>
-      <c r="P47" s="74"/>
-      <c r="Q47" s="74"/>
-      <c r="R47" s="74"/>
-      <c r="S47" s="74"/>
+      <c r="L47" s="71"/>
+      <c r="M47" s="71"/>
+      <c r="N47" s="71"/>
+      <c r="O47" s="71"/>
+      <c r="P47" s="71"/>
+      <c r="Q47" s="71"/>
+      <c r="R47" s="71"/>
+      <c r="S47" s="71"/>
       <c r="T47" s="30"/>
       <c r="U47" s="30"/>
       <c r="V47" s="30"/>
@@ -14499,24 +14523,24 @@
     </row>
     <row r="48" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="30"/>
-      <c r="B48" s="71"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="71"/>
-      <c r="H48" s="71"/>
-      <c r="I48" s="71"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="74"/>
       <c r="J48" s="30"/>
       <c r="K48" s="30"/>
-      <c r="L48" s="74"/>
-      <c r="M48" s="74"/>
-      <c r="N48" s="74"/>
-      <c r="O48" s="74"/>
-      <c r="P48" s="74"/>
-      <c r="Q48" s="74"/>
-      <c r="R48" s="74"/>
-      <c r="S48" s="74"/>
+      <c r="L48" s="71"/>
+      <c r="M48" s="71"/>
+      <c r="N48" s="71"/>
+      <c r="O48" s="71"/>
+      <c r="P48" s="71"/>
+      <c r="Q48" s="71"/>
+      <c r="R48" s="71"/>
+      <c r="S48" s="71"/>
       <c r="T48" s="30"/>
       <c r="U48" s="30"/>
       <c r="V48" s="30"/>
@@ -14530,14 +14554,14 @@
     </row>
     <row r="49" spans="1:29" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="30"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="71"/>
-      <c r="D49" s="71"/>
-      <c r="E49" s="71"/>
-      <c r="F49" s="71"/>
-      <c r="G49" s="71"/>
-      <c r="H49" s="71"/>
-      <c r="I49" s="71"/>
+      <c r="B49" s="74"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="74"/>
+      <c r="E49" s="74"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="74"/>
+      <c r="I49" s="74"/>
       <c r="J49" s="30"/>
       <c r="K49" s="30"/>
       <c r="L49" s="30"/>
@@ -14561,14 +14585,14 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
-      <c r="B50" s="71"/>
-      <c r="C50" s="71"/>
-      <c r="D50" s="71"/>
-      <c r="E50" s="71"/>
-      <c r="F50" s="71"/>
-      <c r="G50" s="71"/>
-      <c r="H50" s="71"/>
-      <c r="I50" s="71"/>
+      <c r="B50" s="74"/>
+      <c r="C50" s="74"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="I50" s="74"/>
       <c r="J50" s="30"/>
       <c r="K50" s="30"/>
       <c r="L50" s="30"/>
@@ -14592,14 +14616,14 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="30"/>
-      <c r="B51" s="71"/>
-      <c r="C51" s="71"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="71"/>
-      <c r="F51" s="71"/>
-      <c r="G51" s="71"/>
-      <c r="H51" s="71"/>
-      <c r="I51" s="71"/>
+      <c r="B51" s="74"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
+      <c r="F51" s="74"/>
+      <c r="G51" s="74"/>
+      <c r="H51" s="74"/>
+      <c r="I51" s="74"/>
       <c r="J51" s="30"/>
       <c r="K51" s="30"/>
       <c r="L51" s="30"/>
@@ -15754,18 +15778,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Ni3oRhRFSHLqcHPeDMM9oJPhO6WfMxTCuA0QUr0aYxZ5GIVg5SnJ0DmCKugqbXaRKsIRpp0xaviZSFtXtsEQYA==" saltValue="uU6zNIz4+Gs4uisLnne5sQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="27">
-    <mergeCell ref="L20:S21"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="V4:AC4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="V5:AC5"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="V7:AC7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="V8:AC8"/>
-    <mergeCell ref="V10:AC10"/>
-    <mergeCell ref="L16:S17"/>
-    <mergeCell ref="L18:S18"/>
     <mergeCell ref="B47:I51"/>
     <mergeCell ref="L23:S24"/>
     <mergeCell ref="B31:I31"/>
@@ -15781,6 +15793,18 @@
     <mergeCell ref="L43:S45"/>
     <mergeCell ref="V44:AC45"/>
     <mergeCell ref="L46:S48"/>
+    <mergeCell ref="L20:S21"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="V4:AC4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="V5:AC5"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="V7:AC7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="V8:AC8"/>
+    <mergeCell ref="V10:AC10"/>
+    <mergeCell ref="L16:S17"/>
+    <mergeCell ref="L18:S18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{5E7C7A05-D050-4790-AD5A-2C904F987D3F}"/>
@@ -15814,49 +15838,49 @@
   <sheetData>
     <row r="1" spans="1:4" s="58" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
-        <v>1172</v>
+        <v>1164</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>1204</v>
+        <v>1196</v>
       </c>
       <c r="C1" s="58" t="s">
-        <v>1173</v>
+        <v>1165</v>
       </c>
       <c r="D1" s="60" t="s">
-        <v>1203</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
-        <v>1174</v>
+        <v>1166</v>
       </c>
       <c r="B2" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="61" t="s">
-        <v>1175</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
-        <v>1176</v>
+        <v>1168</v>
       </c>
       <c r="B3" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="61" t="s">
-        <v>1177</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="s">
-        <v>1178</v>
+        <v>1170</v>
       </c>
       <c r="B4" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>1179</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15867,7 +15891,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>1180</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15878,16 +15902,16 @@
         <v>51</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>1181</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
-        <v>1182</v>
+        <v>1174</v>
       </c>
       <c r="B7" s="57"/>
       <c r="C7" s="63" t="s">
-        <v>1183</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15896,16 +15920,16 @@
       </c>
       <c r="B8" s="57"/>
       <c r="C8" s="63" t="s">
-        <v>1184</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
-        <v>1185</v>
+        <v>1177</v>
       </c>
       <c r="B9" s="57"/>
       <c r="C9" s="63" t="s">
-        <v>1186</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
@@ -15916,7 +15940,7 @@
         <v>51</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>1187</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15927,10 +15951,10 @@
         <v>51</v>
       </c>
       <c r="C11" s="61" t="s">
-        <v>1188</v>
+        <v>1180</v>
       </c>
       <c r="D11" s="62" t="s">
-        <v>1205</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15939,7 +15963,7 @@
       </c>
       <c r="B12" s="57"/>
       <c r="C12" s="63" t="s">
-        <v>1189</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15950,10 +15974,10 @@
         <v>51</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
       <c r="D13" s="62" t="s">
-        <v>1206</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15962,7 +15986,7 @@
       </c>
       <c r="B14" s="57"/>
       <c r="C14" s="63" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15971,7 +15995,7 @@
       </c>
       <c r="B15" s="57"/>
       <c r="C15" s="63" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15980,7 +16004,7 @@
       </c>
       <c r="B16" s="57"/>
       <c r="C16" s="63" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15989,7 +16013,7 @@
       </c>
       <c r="B17" s="57"/>
       <c r="C17" s="63" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -15998,7 +16022,7 @@
       </c>
       <c r="B18" s="57"/>
       <c r="C18" s="63" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -16007,7 +16031,7 @@
       </c>
       <c r="B19" s="57"/>
       <c r="C19" s="63" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -16016,7 +16040,7 @@
       </c>
       <c r="B20" s="57"/>
       <c r="C20" s="63" t="s">
-        <v>1190</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="48" x14ac:dyDescent="0.2">
@@ -16025,21 +16049,21 @@
       </c>
       <c r="B21" s="57"/>
       <c r="C21" s="63" t="s">
-        <v>1191</v>
+        <v>1183</v>
       </c>
       <c r="D21" s="62" t="s">
-        <v>1207</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="55" t="s">
-        <v>1192</v>
+        <v>1184</v>
       </c>
       <c r="B22" s="56" t="s">
         <v>51</v>
       </c>
       <c r="C22" s="61" t="s">
-        <v>1193</v>
+        <v>1185</v>
       </c>
     </row>
   </sheetData>
@@ -16057,7 +16081,7 @@
   <dimension ref="A1:AD63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16120,7 +16144,7 @@
         <v>56</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>1194</v>
+        <v>1186</v>
       </c>
       <c r="J1" s="54" t="s">
         <v>54</v>
@@ -16132,58 +16156,58 @@
         <v>411</v>
       </c>
       <c r="M1" s="54" t="s">
-        <v>57</v>
+        <v>1228</v>
       </c>
       <c r="N1" s="27" t="s">
-        <v>1113</v>
+        <v>1229</v>
       </c>
       <c r="O1" s="34" t="s">
-        <v>58</v>
+        <v>1230</v>
       </c>
       <c r="P1" s="29" t="s">
-        <v>1112</v>
+        <v>1231</v>
       </c>
       <c r="Q1" s="37" t="s">
-        <v>59</v>
+        <v>1232</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>1114</v>
+        <v>1233</v>
       </c>
       <c r="S1" s="36" t="s">
-        <v>60</v>
+        <v>1234</v>
       </c>
       <c r="T1" s="29" t="s">
-        <v>1115</v>
+        <v>1235</v>
       </c>
       <c r="U1" s="36" t="s">
-        <v>61</v>
+        <v>1236</v>
       </c>
       <c r="V1" s="28" t="s">
-        <v>1116</v>
+        <v>1237</v>
       </c>
       <c r="W1" s="36" t="s">
-        <v>62</v>
+        <v>1238</v>
       </c>
       <c r="X1" s="28" t="s">
-        <v>1117</v>
+        <v>1239</v>
       </c>
       <c r="Y1" s="36" t="s">
-        <v>63</v>
+        <v>1240</v>
       </c>
       <c r="Z1" s="28" t="s">
-        <v>1118</v>
+        <v>1241</v>
       </c>
       <c r="AA1" s="36" t="s">
-        <v>64</v>
+        <v>1242</v>
       </c>
       <c r="AB1" s="28" t="s">
-        <v>1119</v>
+        <v>1243</v>
       </c>
       <c r="AC1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="AD1" s="54" t="s">
-        <v>1120</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -19385,7 +19409,7 @@
     <row r="62" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="63" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="V+L/i8oUq04NkKb3zfH4lYeKHQiCTuZI2/jdXoGDvwVIm29mxr5TRP+AArSWO+UWt8mlUT1udm1v3IU4rU59BQ==" saltValue="n/Gc2vQtAj269gutY0hN0Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -19459,7 +19483,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1195</v>
+        <v>1187</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -19500,7 +19524,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1122</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -19508,47 +19532,47 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>1123</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1167</v>
+        <v>1159</v>
       </c>
       <c r="B3" t="s">
-        <v>1124</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
       <c r="B4" t="s">
-        <v>1125</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
       <c r="B5" t="s">
-        <v>1126</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1170</v>
+        <v>1162</v>
       </c>
       <c r="B6" t="s">
-        <v>1127</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1171</v>
+        <v>1163</v>
       </c>
       <c r="B7" t="s">
-        <v>1128</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -19556,7 +19580,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>1129</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -19564,7 +19588,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>1130</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -19572,7 +19596,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>1131</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -19580,7 +19604,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>1132</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -19588,7 +19612,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>1133</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -19596,7 +19620,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>1134</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -19604,7 +19628,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>1135</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -19612,7 +19636,7 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>1136</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -19620,7 +19644,7 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>1137</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -19628,7 +19652,7 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>1138</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -19636,7 +19660,7 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>1139</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -19644,7 +19668,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>1140</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -19652,7 +19676,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>1141</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -19660,7 +19684,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>1142</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -19668,7 +19692,7 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>1143</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -19676,7 +19700,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>1144</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -19684,7 +19708,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>1145</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -19692,7 +19716,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>1146</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -19700,7 +19724,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>1147</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -19708,7 +19732,7 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>1148</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -19716,7 +19740,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>1149</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -19724,7 +19748,7 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>1150</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -19732,7 +19756,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>1151</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -19740,7 +19764,7 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -19748,7 +19772,7 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>1153</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -19756,7 +19780,7 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>1154</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -19764,7 +19788,7 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>1155</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -19772,7 +19796,7 @@
         <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>1156</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -19780,7 +19804,7 @@
         <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>1157</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -19788,7 +19812,7 @@
         <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>1158</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -19796,7 +19820,7 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>1159</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -19804,7 +19828,7 @@
         <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>1160</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -19812,7 +19836,7 @@
         <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>1161</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -19820,7 +19844,7 @@
         <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>1162</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -19828,7 +19852,7 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>1163</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -19836,7 +19860,7 @@
         <v>48</v>
       </c>
       <c r="B43" t="s">
-        <v>1164</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -19844,7 +19868,7 @@
         <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>1165</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -19852,7 +19876,7 @@
         <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>1166</v>
+        <v>1158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>